<commit_message>
convert to xlsx as inputs
</commit_message>
<xml_diff>
--- a/msn/optimized_production.xlsx
+++ b/msn/optimized_production.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1001,6 +1001,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
output of equal allocation
</commit_message>
<xml_diff>
--- a/msn/optimized_production.xlsx
+++ b/msn/optimized_production.xlsx
@@ -513,491 +513,491 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FAP0002</t>
+          <t>FAP0007</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>634</v>
+        <v>831</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>33886</v>
+        <v>32901</v>
       </c>
       <c r="E2" t="n">
-        <v>30044</v>
+        <v>27397</v>
       </c>
       <c r="F2" t="n">
-        <v>30223</v>
+        <v>26745</v>
       </c>
       <c r="G2" t="n">
-        <v>27671</v>
+        <v>27320</v>
       </c>
       <c r="H2" t="n">
-        <v>24700</v>
+        <v>25420</v>
       </c>
       <c r="I2" t="n">
-        <v>27185</v>
+        <v>23510</v>
       </c>
       <c r="J2" t="n">
-        <v>29557</v>
+        <v>27347</v>
       </c>
       <c r="K2" t="n">
-        <v>28411</v>
+        <v>25567</v>
       </c>
       <c r="L2" t="n">
-        <v>26621</v>
+        <v>23777</v>
       </c>
       <c r="M2" t="n">
-        <v>32991</v>
+        <v>32049</v>
       </c>
       <c r="N2" t="n">
-        <v>31137</v>
+        <v>31026</v>
       </c>
       <c r="O2" t="n">
-        <v>31159</v>
+        <v>27681</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FAP0003</t>
+          <t>FAP0009</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>860</v>
+        <v>831</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>27866</v>
+        <v>27915</v>
       </c>
       <c r="E3" t="n">
-        <v>23164</v>
+        <v>19918</v>
       </c>
       <c r="F3" t="n">
-        <v>25923</v>
+        <v>21759</v>
       </c>
       <c r="G3" t="n">
-        <v>23371</v>
+        <v>19841</v>
       </c>
       <c r="H3" t="n">
-        <v>17820</v>
+        <v>17941</v>
       </c>
       <c r="I3" t="n">
-        <v>21165</v>
+        <v>18524</v>
       </c>
       <c r="J3" t="n">
-        <v>23537</v>
+        <v>22361</v>
       </c>
       <c r="K3" t="n">
-        <v>24111</v>
+        <v>19750</v>
       </c>
       <c r="L3" t="n">
-        <v>21461</v>
+        <v>18791</v>
       </c>
       <c r="M3" t="n">
-        <v>26971</v>
+        <v>25401</v>
       </c>
       <c r="N3" t="n">
-        <v>25117</v>
+        <v>24378</v>
       </c>
       <c r="O3" t="n">
-        <v>23419</v>
+        <v>21033</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FAP0004</t>
+          <t>FAP0010</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>924</v>
+        <v>831</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="D4" t="n">
-        <v>22322</v>
+        <v>22098</v>
       </c>
       <c r="E4" t="n">
-        <v>14848</v>
+        <v>12439</v>
       </c>
       <c r="F4" t="n">
-        <v>21303</v>
+        <v>15942</v>
       </c>
       <c r="G4" t="n">
-        <v>15979</v>
+        <v>15686</v>
       </c>
       <c r="H4" t="n">
-        <v>12276</v>
+        <v>12955</v>
       </c>
       <c r="I4" t="n">
-        <v>16545</v>
+        <v>14369</v>
       </c>
       <c r="J4" t="n">
-        <v>17993</v>
+        <v>17375</v>
       </c>
       <c r="K4" t="n">
-        <v>18567</v>
+        <v>14764</v>
       </c>
       <c r="L4" t="n">
-        <v>16841</v>
+        <v>14636</v>
       </c>
       <c r="M4" t="n">
-        <v>18655</v>
+        <v>19584</v>
       </c>
       <c r="N4" t="n">
-        <v>18649</v>
+        <v>17730</v>
       </c>
       <c r="O4" t="n">
-        <v>17875</v>
+        <v>16047</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FAP0005</t>
+          <t>FAP0008</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>538</v>
+        <v>892</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>19094</v>
+        <v>14962</v>
       </c>
       <c r="E5" t="n">
-        <v>10006</v>
+        <v>6195</v>
       </c>
       <c r="F5" t="n">
-        <v>18075</v>
+        <v>10590</v>
       </c>
       <c r="G5" t="n">
-        <v>12751</v>
+        <v>11226</v>
       </c>
       <c r="H5" t="n">
-        <v>9048</v>
+        <v>7603</v>
       </c>
       <c r="I5" t="n">
-        <v>13855</v>
+        <v>7233</v>
       </c>
       <c r="J5" t="n">
-        <v>13689</v>
+        <v>12023</v>
       </c>
       <c r="K5" t="n">
-        <v>14801</v>
+        <v>9412</v>
       </c>
       <c r="L5" t="n">
-        <v>11999</v>
+        <v>7500</v>
       </c>
       <c r="M5" t="n">
-        <v>15427</v>
+        <v>14232</v>
       </c>
       <c r="N5" t="n">
-        <v>15959</v>
+        <v>13270</v>
       </c>
       <c r="O5" t="n">
-        <v>13571</v>
+        <v>8911</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FAP0006</t>
+          <t>FAP0001</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>965</v>
+        <v>774</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D6" t="n">
-        <v>14269</v>
+        <v>10318</v>
       </c>
       <c r="E6" t="n">
-        <v>3251</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
-        <v>12285</v>
+        <v>4398</v>
       </c>
       <c r="G6" t="n">
-        <v>4066</v>
+        <v>5034</v>
       </c>
       <c r="H6" t="n">
-        <v>4223</v>
+        <v>2959</v>
       </c>
       <c r="I6" t="n">
-        <v>5170</v>
+        <v>3363</v>
       </c>
       <c r="J6" t="n">
-        <v>7899</v>
+        <v>8153</v>
       </c>
       <c r="K6" t="n">
-        <v>7081</v>
+        <v>4768</v>
       </c>
       <c r="L6" t="n">
-        <v>5244</v>
+        <v>3630</v>
       </c>
       <c r="M6" t="n">
-        <v>10602</v>
+        <v>9588</v>
       </c>
       <c r="N6" t="n">
-        <v>7274</v>
+        <v>7078</v>
       </c>
       <c r="O6" t="n">
-        <v>7781</v>
+        <v>4267</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FAP0001</t>
+          <t>FAP0002</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>406</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>568</v>
+        <v>634</v>
       </c>
       <c r="D7" t="n">
-        <v>11833</v>
+        <v>10318</v>
       </c>
       <c r="E7" t="n">
         <v>3</v>
       </c>
       <c r="F7" t="n">
-        <v>9037</v>
+        <v>4398</v>
       </c>
       <c r="G7" t="n">
-        <v>818</v>
+        <v>5034</v>
       </c>
       <c r="H7" t="n">
-        <v>1787</v>
+        <v>2959</v>
       </c>
       <c r="I7" t="n">
-        <v>3140</v>
+        <v>3363</v>
       </c>
       <c r="J7" t="n">
-        <v>5869</v>
+        <v>8153</v>
       </c>
       <c r="K7" t="n">
-        <v>4645</v>
+        <v>4768</v>
       </c>
       <c r="L7" t="n">
-        <v>3214</v>
+        <v>3630</v>
       </c>
       <c r="M7" t="n">
-        <v>8166</v>
+        <v>9588</v>
       </c>
       <c r="N7" t="n">
-        <v>4026</v>
+        <v>7078</v>
       </c>
       <c r="O7" t="n">
-        <v>5345</v>
+        <v>4267</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>FAP0008</t>
+          <t>FAP0003</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>892</v>
+        <v>860</v>
       </c>
       <c r="D8" t="n">
-        <v>11833</v>
+        <v>10318</v>
       </c>
       <c r="E8" t="n">
         <v>3</v>
       </c>
       <c r="F8" t="n">
-        <v>9037</v>
+        <v>4398</v>
       </c>
       <c r="G8" t="n">
-        <v>818</v>
+        <v>5034</v>
       </c>
       <c r="H8" t="n">
-        <v>1787</v>
+        <v>2959</v>
       </c>
       <c r="I8" t="n">
-        <v>3140</v>
+        <v>3363</v>
       </c>
       <c r="J8" t="n">
-        <v>5869</v>
+        <v>8153</v>
       </c>
       <c r="K8" t="n">
-        <v>4645</v>
+        <v>4768</v>
       </c>
       <c r="L8" t="n">
-        <v>3214</v>
+        <v>3630</v>
       </c>
       <c r="M8" t="n">
-        <v>8166</v>
+        <v>9588</v>
       </c>
       <c r="N8" t="n">
-        <v>4026</v>
+        <v>7078</v>
       </c>
       <c r="O8" t="n">
-        <v>5345</v>
+        <v>4267</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FAP0007</t>
+          <t>FAP0004</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>853</v>
+        <v>924</v>
       </c>
       <c r="D9" t="n">
-        <v>11833</v>
+        <v>10318</v>
       </c>
       <c r="E9" t="n">
         <v>3</v>
       </c>
       <c r="F9" t="n">
-        <v>9037</v>
+        <v>4398</v>
       </c>
       <c r="G9" t="n">
-        <v>818</v>
+        <v>5034</v>
       </c>
       <c r="H9" t="n">
-        <v>1787</v>
+        <v>2959</v>
       </c>
       <c r="I9" t="n">
-        <v>3140</v>
+        <v>3363</v>
       </c>
       <c r="J9" t="n">
-        <v>5869</v>
+        <v>8153</v>
       </c>
       <c r="K9" t="n">
-        <v>4645</v>
+        <v>4768</v>
       </c>
       <c r="L9" t="n">
-        <v>3214</v>
+        <v>3630</v>
       </c>
       <c r="M9" t="n">
-        <v>8166</v>
+        <v>9588</v>
       </c>
       <c r="N9" t="n">
-        <v>4026</v>
+        <v>7078</v>
       </c>
       <c r="O9" t="n">
-        <v>5345</v>
+        <v>4267</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>FAP0009</t>
+          <t>FAP0005</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>831</v>
+        <v>538</v>
       </c>
       <c r="D10" t="n">
-        <v>11833</v>
+        <v>10318</v>
       </c>
       <c r="E10" t="n">
         <v>3</v>
       </c>
       <c r="F10" t="n">
-        <v>9037</v>
+        <v>4398</v>
       </c>
       <c r="G10" t="n">
-        <v>818</v>
+        <v>5034</v>
       </c>
       <c r="H10" t="n">
-        <v>1787</v>
+        <v>2959</v>
       </c>
       <c r="I10" t="n">
-        <v>3140</v>
+        <v>3363</v>
       </c>
       <c r="J10" t="n">
-        <v>5869</v>
+        <v>8153</v>
       </c>
       <c r="K10" t="n">
-        <v>4645</v>
+        <v>4768</v>
       </c>
       <c r="L10" t="n">
-        <v>3214</v>
+        <v>3630</v>
       </c>
       <c r="M10" t="n">
-        <v>8166</v>
+        <v>9588</v>
       </c>
       <c r="N10" t="n">
-        <v>4026</v>
+        <v>7078</v>
       </c>
       <c r="O10" t="n">
-        <v>5345</v>
+        <v>4267</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>FAP0010</t>
+          <t>FAP0006</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>950</v>
+        <v>965</v>
       </c>
       <c r="D11" t="n">
-        <v>11833</v>
+        <v>10318</v>
       </c>
       <c r="E11" t="n">
         <v>3</v>
       </c>
       <c r="F11" t="n">
-        <v>9037</v>
+        <v>4398</v>
       </c>
       <c r="G11" t="n">
-        <v>818</v>
+        <v>5034</v>
       </c>
       <c r="H11" t="n">
-        <v>1787</v>
+        <v>2959</v>
       </c>
       <c r="I11" t="n">
-        <v>3140</v>
+        <v>3363</v>
       </c>
       <c r="J11" t="n">
-        <v>5869</v>
+        <v>8153</v>
       </c>
       <c r="K11" t="n">
-        <v>4645</v>
+        <v>4768</v>
       </c>
       <c r="L11" t="n">
-        <v>3214</v>
+        <v>3630</v>
       </c>
       <c r="M11" t="n">
-        <v>8166</v>
+        <v>9588</v>
       </c>
       <c r="N11" t="n">
-        <v>4026</v>
+        <v>7078</v>
       </c>
       <c r="O11" t="n">
-        <v>5345</v>
+        <v>4267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>